<commit_message>
number and amount check
</commit_message>
<xml_diff>
--- a/nonhistory.xlsx
+++ b/nonhistory.xlsx
@@ -31,19 +31,19 @@
     <t>Date</t>
   </si>
   <si>
-    <t>history test</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
-    <t>1222</t>
-  </si>
-  <si>
-    <t>23</t>
-  </si>
-  <si>
-    <t>27/10/2022 22:12:25</t>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>3354</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>28/10/2022 20:21:14</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
last day of month and column width resolved
</commit_message>
<xml_diff>
--- a/nonhistory.xlsx
+++ b/nonhistory.xlsx
@@ -31,19 +31,19 @@
     <t>Date</t>
   </si>
   <si>
-    <t>test</t>
-  </si>
-  <si>
-    <t>ref</t>
-  </si>
-  <si>
-    <t>3354</t>
-  </si>
-  <si>
-    <t>56</t>
-  </si>
-  <si>
-    <t>28/10/2022 20:21:14</t>
+    <t>dada life</t>
+  </si>
+  <si>
+    <t>violents1</t>
+  </si>
+  <si>
+    <t>2321</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>31/10/2022 20:42:56</t>
   </si>
 </sst>
 </file>
@@ -406,6 +406,13 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="6.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">

</xml_diff>